<commit_message>
modified edit_question, add delete_question.php
</commit_message>
<xml_diff>
--- a/@Table Schema and work priority.xlsx
+++ b/@Table Schema and work priority.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24620" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>Questions</t>
   </si>
   <si>
-    <t>Quizzes</t>
-  </si>
-  <si>
     <t>Leaderboards</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>category_id</t>
+  </si>
+  <si>
+    <t>Quiz</t>
   </si>
 </sst>
 </file>
@@ -336,8 +336,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -389,20 +391,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -414,6 +416,7 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -425,6 +428,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -756,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -775,12 +779,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:20" ht="12.75" customHeight="1">
       <c r="A2" s="7"/>
@@ -797,15 +801,15 @@
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -819,27 +823,27 @@
     <row r="3" spans="1:20" ht="12.75" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -852,216 +856,216 @@
     </row>
     <row r="4" spans="1:20" ht="12.75" customHeight="1">
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
         <v>8</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="12.75" customHeight="1">
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>13</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="12.75" customHeight="1">
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="12.75" customHeight="1">
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H7" s="3"/>
       <c r="J7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="12.75" customHeight="1">
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="12.75" customHeight="1">
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
         <v>21</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="12.75" customHeight="1">
       <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>63</v>
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="12.75" customHeight="1">
       <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="12.75" customHeight="1">
       <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="12.75" customHeight="1">
       <c r="F13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="12.75" customHeight="1">
       <c r="B14" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="12.75" customHeight="1">
       <c r="B15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="12.75" customHeight="1">
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:20" ht="12.75" customHeight="1">
       <c r="F17" s="12"/>
       <c r="H17" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:20" ht="12.75" customHeight="1">
       <c r="F18" s="12"/>
       <c r="H18" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:20" ht="12.75" customHeight="1">
       <c r="H19" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="12.75" customHeight="1">
       <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
         <v>35</v>
-      </c>
-      <c r="H20" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:20" ht="12.75" customHeight="1">
       <c r="F21" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:20" ht="12.75" customHeight="1">
       <c r="F22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="2:20" ht="12" customHeight="1">
       <c r="F23" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:20" ht="12.75" customHeight="1">
       <c r="E24" s="8"/>
       <c r="F24" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -1080,174 +1084,173 @@
     </row>
     <row r="26" spans="2:20" ht="14" customHeight="1"/>
     <row r="27" spans="2:20" ht="49" customHeight="1">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="2:20" ht="12.75" customHeight="1">
+      <c r="B28" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="2:20" ht="12.75" customHeight="1">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="8"/>
+      <c r="D28" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8" t="s">
+    </row>
+    <row r="29" spans="2:20" ht="12.75" customHeight="1">
+      <c r="B29" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="2:20" ht="12.75" customHeight="1">
-      <c r="C29" s="6" t="s">
+      <c r="C29" t="s">
         <v>42</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" ht="12.75" customHeight="1">
+      <c r="B30" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E29">
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="12.75" customHeight="1">
-      <c r="C30" s="6" t="s">
+    <row r="31" spans="2:20" ht="12.75" customHeight="1">
+      <c r="B31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D30" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30">
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="12.75" customHeight="1">
-      <c r="C31" s="6" t="s">
+    <row r="32" spans="2:20" ht="12.75" customHeight="1">
+      <c r="B32" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31">
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="12.75" customHeight="1">
-      <c r="C32" s="6" t="s">
+    <row r="33" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B33" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D32" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32">
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="3:5" ht="12.75" customHeight="1">
-      <c r="C33" s="6" t="s">
+    <row r="34" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B34" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" ht="12.75" customHeight="1">
-      <c r="C34" s="4" t="s">
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B35" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D34" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34">
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="3:5" ht="12.75" customHeight="1">
-      <c r="C35" s="4" t="s">
+    <row r="36" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B36" t="s">
         <v>49</v>
       </c>
-      <c r="D35" t="s">
-        <v>43</v>
-      </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" ht="12.75" customHeight="1">
       <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B37" t="s">
         <v>50</v>
       </c>
-      <c r="D36" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36">
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="3:5" ht="12.75" customHeight="1">
-      <c r="C37" t="s">
+    <row r="38" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B38" t="s">
         <v>51</v>
       </c>
-      <c r="D37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37">
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="3:5" ht="12.75" customHeight="1">
-      <c r="C38" t="s">
+    <row r="39" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B39" t="s">
         <v>52</v>
       </c>
-      <c r="D38" t="s">
-        <v>43</v>
-      </c>
-      <c r="E38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" ht="12.75" customHeight="1">
       <c r="C39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B40" t="s">
         <v>53</v>
       </c>
-      <c r="D39" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39">
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="3:5" ht="12.75" customHeight="1">
-      <c r="C40" t="s">
+    <row r="41" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B41" t="s">
         <v>54</v>
       </c>
-      <c r="D40" t="s">
-        <v>43</v>
-      </c>
-      <c r="E40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" ht="12.75" customHeight="1">
       <c r="C41" t="s">
         <v>55</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="12.75" customHeight="1">
+      <c r="B42" t="s">
         <v>56</v>
       </c>
-      <c r="E41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5" ht="12.75" customHeight="1">
       <c r="C42" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42">
+        <v>55</v>
+      </c>
+      <c r="D42">
         <v>4</v>
       </c>
     </row>

</xml_diff>